<commit_message>
Agrego anotaciones del excel segun lo hablado en la llamada
</commit_message>
<xml_diff>
--- a/tp5/PIZZERIA/draft/tp5.xlsx
+++ b/tp5/PIZZERIA/draft/tp5.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mati\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3543C611-DE8E-453D-9CA0-555BB40F13BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="104">
   <si>
     <t>Evento</t>
   </si>
@@ -242,9 +236,6 @@
     <t>Pedidos para entregar</t>
   </si>
   <si>
-    <t>12*3,5+1*2,5</t>
-  </si>
-  <si>
     <t>sw</t>
   </si>
   <si>
@@ -315,13 +306,46 @@
   </si>
   <si>
     <t>fin entrega</t>
+  </si>
+  <si>
+    <t>Empleado1</t>
+  </si>
+  <si>
+    <t>Llegada_pedido</t>
+  </si>
+  <si>
+    <t>4*3,5+1*2,5</t>
+  </si>
+  <si>
+    <t>mañana</t>
+  </si>
+  <si>
+    <t>Se tira al finalizar el turno</t>
+  </si>
+  <si>
+    <t>Pregunta si hay en stock y si no pregunta por estados de empleados</t>
+  </si>
+  <si>
+    <t>si es mas de una hora se almacena</t>
+  </si>
+  <si>
+    <t>Se pierde Cliente?</t>
+  </si>
+  <si>
+    <t>si la demora es mas de una hora se descarta y se pierde el cliente</t>
+  </si>
+  <si>
+    <t>va a cola?</t>
+  </si>
+  <si>
+    <t>Se atienden todos despues de finalizar el turno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -524,6 +548,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -539,8 +584,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -554,26 +599,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -635,7 +668,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -667,27 +700,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -719,24 +734,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -912,51 +909,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:BQ20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:BR26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="12" max="13" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" customWidth="1"/>
-    <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" customWidth="1"/>
-    <col min="22" max="22" width="17.42578125" customWidth="1"/>
-    <col min="23" max="23" width="15.5703125" customWidth="1"/>
-    <col min="25" max="25" width="13.140625" customWidth="1"/>
-    <col min="26" max="27" width="14.7109375" customWidth="1"/>
-    <col min="28" max="28" width="28.5703125" customWidth="1"/>
-    <col min="29" max="29" width="15.42578125" customWidth="1"/>
-    <col min="30" max="30" width="14.28515625" customWidth="1"/>
-    <col min="31" max="31" width="17" customWidth="1"/>
-    <col min="32" max="32" width="15.42578125" customWidth="1"/>
-    <col min="33" max="33" width="16.85546875" customWidth="1"/>
-    <col min="34" max="34" width="13.42578125" customWidth="1"/>
-    <col min="35" max="35" width="13.5703125" customWidth="1"/>
-    <col min="38" max="38" width="25.28515625" customWidth="1"/>
-    <col min="40" max="40" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="41.42578125" customWidth="1"/>
-    <col min="44" max="44" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="25.42578125" customWidth="1"/>
-    <col min="47" max="47" width="15" customWidth="1"/>
-    <col min="49" max="49" width="22.7109375" customWidth="1"/>
-    <col min="50" max="50" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.140625" customWidth="1"/>
+    <col min="13" max="14" width="13.5703125" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="14" customWidth="1"/>
+    <col min="18" max="18" width="18.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" customWidth="1"/>
+    <col min="23" max="23" width="17.42578125" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" customWidth="1"/>
+    <col min="26" max="26" width="13.140625" customWidth="1"/>
+    <col min="27" max="27" width="14.7109375" customWidth="1"/>
+    <col min="28" max="28" width="18.7109375" customWidth="1"/>
+    <col min="29" max="29" width="28.5703125" customWidth="1"/>
+    <col min="30" max="30" width="15.42578125" customWidth="1"/>
+    <col min="31" max="31" width="14.28515625" customWidth="1"/>
+    <col min="32" max="32" width="17" customWidth="1"/>
+    <col min="33" max="33" width="15.42578125" customWidth="1"/>
+    <col min="34" max="34" width="16.85546875" customWidth="1"/>
+    <col min="35" max="35" width="13.42578125" customWidth="1"/>
+    <col min="36" max="36" width="13.5703125" customWidth="1"/>
+    <col min="39" max="39" width="14" customWidth="1"/>
+    <col min="41" max="41" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="41.42578125" customWidth="1"/>
+    <col min="45" max="45" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="25.42578125" customWidth="1"/>
+    <col min="48" max="48" width="15" customWidth="1"/>
+    <col min="50" max="50" width="22.7109375" customWidth="1"/>
+    <col min="51" max="51" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:70">
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -972,30 +971,30 @@
       <c r="J2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="6"/>
-      <c r="O2" s="5" t="s">
+      <c r="N2" s="6"/>
+      <c r="P2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>26</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:70">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1011,20 +1010,20 @@
       <c r="J3" s="1">
         <v>0.2</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>19</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>38</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>27</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:70">
       <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1037,20 +1036,20 @@
       <c r="J4" s="1">
         <v>0.4</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>55</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="S4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>39</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:70">
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1066,11 +1065,11 @@
       <c r="J5" s="1">
         <v>0.3</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:70">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1086,11 +1085,11 @@
       <c r="J6" s="1">
         <v>0.05</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:70">
       <c r="G7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1104,123 +1103,126 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="2:69" x14ac:dyDescent="0.25">
-      <c r="AO8" t="s">
+    <row r="8" spans="2:70">
+      <c r="AP8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>77</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="2:70">
+      <c r="B9" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD9" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE9" s="25"/>
+      <c r="AF9" s="25"/>
+      <c r="AG9" s="25"/>
+      <c r="AH9" s="25"/>
+      <c r="AI9" s="26"/>
+      <c r="AJ9" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK9" s="20"/>
+      <c r="AL9" s="20"/>
+      <c r="AM9" s="20"/>
+      <c r="AN9" s="20"/>
+      <c r="AO9" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP9" s="33"/>
+      <c r="AQ9" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR9" s="34"/>
+      <c r="AS9" s="33"/>
+      <c r="AT9" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU9" s="20"/>
+      <c r="AV9" s="20"/>
+      <c r="AW9" s="20"/>
+      <c r="AX9" s="20"/>
+      <c r="AY9" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="AZ9" s="20"/>
+      <c r="BA9" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="BB9" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="BC9" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="BJ9" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK9" s="13"/>
+      <c r="BL9" s="13"/>
+      <c r="BM9" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="AP8" t="s">
-        <v>78</v>
-      </c>
-      <c r="BB8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="2:69" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="17"/>
-      <c r="W9" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="18"/>
-      <c r="AA9" s="18"/>
-      <c r="AB9" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC9" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="16"/>
-      <c r="AF9" s="16"/>
-      <c r="AG9" s="16"/>
-      <c r="AH9" s="17"/>
-      <c r="AI9" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ9" s="18"/>
-      <c r="AK9" s="18"/>
-      <c r="AL9" s="18"/>
-      <c r="AM9" s="18"/>
-      <c r="AN9" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="AO9" s="26"/>
-      <c r="AP9" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="AQ9" s="28"/>
-      <c r="AR9" s="26"/>
-      <c r="AS9" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="AT9" s="18"/>
-      <c r="AU9" s="18"/>
-      <c r="AV9" s="18"/>
-      <c r="AW9" s="18"/>
-      <c r="AX9" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="AY9" s="18"/>
-      <c r="AZ9" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="BA9" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="BB9" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="BI9" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="BJ9" s="23"/>
-      <c r="BK9" s="23"/>
-      <c r="BL9" s="23" t="s">
+      <c r="BN9" s="13"/>
+      <c r="BO9" s="13"/>
+      <c r="BP9" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="BM9" s="23"/>
-      <c r="BN9" s="23"/>
-      <c r="BO9" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="BP9" s="23"/>
-      <c r="BQ9" s="23"/>
-    </row>
-    <row r="10" spans="2:69" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
+      <c r="BQ9" s="13"/>
+      <c r="BR9" s="13"/>
+    </row>
+    <row r="10" spans="2:70" ht="35.25" customHeight="1">
+      <c r="B10" s="23"/>
       <c r="C10" s="8" t="s">
         <v>1</v>
       </c>
@@ -1248,152 +1250,155 @@
       <c r="K10" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="L10" s="14"/>
-      <c r="M10" s="8" t="s">
+      <c r="L10" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="M10" s="23"/>
+      <c r="N10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="N10" s="8" t="s">
+      <c r="O10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O10" s="8" t="s">
+      <c r="P10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="Q10" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="Q10" s="12" t="s">
+      <c r="R10" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="S10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="T10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="U10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="V10" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="W10" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="X10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA10" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB10" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC10" s="31"/>
+      <c r="AD10" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH10" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="R10" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="S10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="T10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="U10" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="V10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="W10" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="X10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z10" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB10" s="22"/>
-      <c r="AC10" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH10" s="9" t="s">
+      <c r="AI10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AI10" s="8" t="s">
+      <c r="AJ10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AJ10" s="8" t="s">
+      <c r="AK10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AK10" s="8" t="s">
+      <c r="AL10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AL10" s="8" t="s">
+      <c r="AM10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AM10" s="8" t="s">
+      <c r="AN10" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AN10" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO10" s="24"/>
-      <c r="AP10" s="24" t="s">
+      <c r="AO10" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP10" s="14"/>
+      <c r="AQ10" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR10" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS10" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="AQ10" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="AR10" s="24" t="s">
+      <c r="AT10" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="AS10" s="11" t="s">
+      <c r="AU10" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="AT10" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="AU10" s="11" t="s">
+      <c r="AV10" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AW10" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="AV10" s="11" t="s">
+      <c r="AX10" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="AW10" s="11" t="s">
+      <c r="AY10" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="AX10" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="AY10" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="AZ10" s="31"/>
-      <c r="BA10" s="30"/>
-      <c r="BB10" s="30"/>
-      <c r="BI10" s="8" t="s">
+      <c r="AZ10" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="BA10" s="21"/>
+      <c r="BB10" s="27"/>
+      <c r="BC10" s="27"/>
+      <c r="BJ10" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="BJ10" s="8" t="s">
+      <c r="BK10" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="BK10" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BL10" s="11" t="s">
+      <c r="BL10" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="BM10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="BM10" s="11" t="s">
+      <c r="BN10" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="BN10" s="11" t="s">
-        <v>93</v>
-      </c>
       <c r="BO10" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="BP10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="BP10" s="11" t="s">
+      <c r="BQ10" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="BQ10" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="2:69" x14ac:dyDescent="0.25">
+      <c r="BR10" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="2:70">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -1406,29 +1411,29 @@
       <c r="K11">
         <v>13</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>0</v>
       </c>
-      <c r="O11" t="s">
-        <v>69</v>
-      </c>
-      <c r="P11">
+      <c r="P11" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q11">
         <v>3.5</v>
       </c>
-      <c r="AB11" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC11">
+      <c r="AC11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD11">
         <v>4</v>
       </c>
-      <c r="AN11">
+      <c r="AO11">
         <v>1</v>
       </c>
-      <c r="AO11">
+      <c r="AP11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:70">
       <c r="B12" t="s">
         <v>66</v>
       </c>
@@ -1436,19 +1441,19 @@
         <v>3.5</v>
       </c>
       <c r="J12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
-      <c r="AN12">
+      <c r="AO12">
         <v>3</v>
       </c>
-      <c r="AO12">
+      <c r="AP12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:70">
       <c r="B13" t="s">
         <v>66</v>
       </c>
@@ -1458,49 +1463,104 @@
       <c r="K13">
         <v>1</v>
       </c>
-      <c r="AN13">
+      <c r="AM13">
+        <v>1</v>
+      </c>
+      <c r="AO13">
         <v>7</v>
       </c>
-      <c r="AO13">
-        <f>AO12+(AN13-AN12)</f>
+      <c r="AP13">
+        <f>AP12+(AO13-AO12)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:69" x14ac:dyDescent="0.25">
-      <c r="AN14">
+    <row r="14" spans="2:70">
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14">
+        <v>45</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>96</v>
+      </c>
+      <c r="AO14">
         <v>7</v>
       </c>
-      <c r="AO14">
-        <f>AO13+(AN14-AN13)</f>
+      <c r="AP14">
+        <f>AP13+(AO14-AO13)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="35:44" x14ac:dyDescent="0.25">
-      <c r="AI18" s="10"/>
-    </row>
-    <row r="20" spans="35:44" x14ac:dyDescent="0.25">
-      <c r="AR20" s="27"/>
+    <row r="15" spans="2:70" ht="169.5" customHeight="1">
+      <c r="L15" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="M15" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="R15" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="U15" s="19"/>
+      <c r="W15" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z15" s="19"/>
+      <c r="AB15" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH15" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="AJ15" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK15" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL15" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM15" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="AN15" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="14:45">
+      <c r="AJ18" s="10"/>
+    </row>
+    <row r="20" spans="14:45">
+      <c r="AS20" s="15"/>
+    </row>
+    <row r="26" spans="14:45">
+      <c r="N26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AN9:AO9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AS9:AW9"/>
-    <mergeCell ref="AX9:AY9"/>
-    <mergeCell ref="AZ9:AZ10"/>
-    <mergeCell ref="BA9:BA10"/>
     <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="W9:AA9"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="X9:AB9"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="I9:K9"/>
-    <mergeCell ref="AI9:AM9"/>
-    <mergeCell ref="M9:Q9"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AH9"/>
+    <mergeCell ref="AJ9:AN9"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AI9"/>
+    <mergeCell ref="AO9:AP9"/>
+    <mergeCell ref="AQ9:AS9"/>
+    <mergeCell ref="AT9:AX9"/>
+    <mergeCell ref="AY9:AZ9"/>
+    <mergeCell ref="BA9:BA10"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="R9:V9"/>
-    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="S9:W9"/>
+    <mergeCell ref="M9:M10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1508,24 +1568,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add tipos de pedidos
</commit_message>
<xml_diff>
--- a/tp5/PIZZERIA/draft/tp5.xlsx
+++ b/tp5/PIZZERIA/draft/tp5.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\note\Desktop\GRtp2\sim2020\tp5\PIZZERIA\draft\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="107">
   <si>
     <t>Evento</t>
   </si>
@@ -339,13 +344,22 @@
   </si>
   <si>
     <t>Se atienden todos despues de finalizar el turno</t>
+  </si>
+  <si>
+    <t>prob Ac</t>
+  </si>
+  <si>
+    <t>int inf</t>
+  </si>
+  <si>
+    <t>int sup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -566,6 +580,42 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -575,37 +625,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -668,7 +689,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -700,9 +721,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -734,6 +756,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -909,14 +932,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BR26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" customWidth="1"/>
@@ -955,10 +978,13 @@
     <col min="54" max="54" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:70">
+    <row r="2" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
@@ -971,8 +997,14 @@
       <c r="J2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>18</v>
+      <c r="K2" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>106</v>
       </c>
       <c r="N2" s="6"/>
       <c r="P2" s="5" t="s">
@@ -994,10 +1026,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:70">
+    <row r="3" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1010,8 +1045,15 @@
       <c r="J3" s="1">
         <v>0.2</v>
       </c>
-      <c r="M3" t="s">
-        <v>19</v>
+      <c r="K3" s="36">
+        <f>SUM(J$3:J3)</f>
+        <v>0.2</v>
+      </c>
+      <c r="L3" s="37">
+        <v>0</v>
+      </c>
+      <c r="M3" s="37">
+        <v>0.19</v>
       </c>
       <c r="Q3" t="s">
         <v>38</v>
@@ -1023,7 +1065,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:70">
+    <row r="4" spans="2:70" x14ac:dyDescent="0.25">
       <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1036,6 +1078,16 @@
       <c r="J4" s="1">
         <v>0.4</v>
       </c>
+      <c r="K4" s="36">
+        <f>SUM(J$3:J4)</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="L4" s="37">
+        <v>0.2</v>
+      </c>
+      <c r="M4" s="37">
+        <v>0.59</v>
+      </c>
       <c r="Q4" t="s">
         <v>55</v>
       </c>
@@ -1049,7 +1101,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:70">
+    <row r="5" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1065,11 +1117,21 @@
       <c r="J5" s="1">
         <v>0.3</v>
       </c>
+      <c r="K5" s="36">
+        <f>SUM(J$3:J5)</f>
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="L5" s="36">
+        <v>0.6</v>
+      </c>
+      <c r="M5" s="37">
+        <v>0.89</v>
+      </c>
       <c r="Q5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:70">
+    <row r="6" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1085,11 +1147,21 @@
       <c r="J6" s="1">
         <v>0.05</v>
       </c>
+      <c r="K6" s="36">
+        <f>SUM(J$3:J6)</f>
+        <v>0.95000000000000018</v>
+      </c>
+      <c r="L6" s="37">
+        <v>0.9</v>
+      </c>
+      <c r="M6" s="37">
+        <v>0.94</v>
+      </c>
       <c r="Q6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:70">
+    <row r="7" spans="2:70" x14ac:dyDescent="0.25">
       <c r="G7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1102,8 +1174,18 @@
       <c r="J7" s="1">
         <v>0.05</v>
       </c>
+      <c r="K7" s="36">
+        <f>SUM(J$3:J7)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="L7" s="37">
+        <v>0.95</v>
+      </c>
+      <c r="M7" s="37">
+        <v>0.99</v>
+      </c>
     </row>
-    <row r="8" spans="2:70">
+    <row r="8" spans="2:70" x14ac:dyDescent="0.25">
       <c r="AP8" t="s">
         <v>72</v>
       </c>
@@ -1114,95 +1196,95 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="2:70">
-      <c r="B9" s="22" t="s">
+    <row r="9" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20" t="s">
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20" t="s">
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
       <c r="L9" s="18"/>
-      <c r="M9" s="22" t="s">
+      <c r="M9" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="28" t="s">
+      <c r="N9" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="24" t="s">
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="25"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="20" t="s">
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Y9" s="20"/>
-      <c r="Z9" s="20"/>
-      <c r="AA9" s="20"/>
-      <c r="AB9" s="20"/>
-      <c r="AC9" s="30" t="s">
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="AD9" s="24" t="s">
+      <c r="AD9" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="AE9" s="25"/>
-      <c r="AF9" s="25"/>
-      <c r="AG9" s="25"/>
-      <c r="AH9" s="25"/>
-      <c r="AI9" s="26"/>
-      <c r="AJ9" s="20" t="s">
+      <c r="AE9" s="28"/>
+      <c r="AF9" s="28"/>
+      <c r="AG9" s="28"/>
+      <c r="AH9" s="28"/>
+      <c r="AI9" s="29"/>
+      <c r="AJ9" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="AK9" s="20"/>
-      <c r="AL9" s="20"/>
-      <c r="AM9" s="20"/>
-      <c r="AN9" s="20"/>
-      <c r="AO9" s="32" t="s">
+      <c r="AK9" s="22"/>
+      <c r="AL9" s="22"/>
+      <c r="AM9" s="22"/>
+      <c r="AN9" s="22"/>
+      <c r="AO9" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="AP9" s="33"/>
-      <c r="AQ9" s="32" t="s">
+      <c r="AP9" s="31"/>
+      <c r="AQ9" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="AR9" s="34"/>
-      <c r="AS9" s="33"/>
-      <c r="AT9" s="20" t="s">
+      <c r="AR9" s="32"/>
+      <c r="AS9" s="31"/>
+      <c r="AT9" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="AU9" s="20"/>
-      <c r="AV9" s="20"/>
-      <c r="AW9" s="20"/>
-      <c r="AX9" s="20"/>
-      <c r="AY9" s="20" t="s">
+      <c r="AU9" s="22"/>
+      <c r="AV9" s="22"/>
+      <c r="AW9" s="22"/>
+      <c r="AX9" s="22"/>
+      <c r="AY9" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="AZ9" s="20"/>
-      <c r="BA9" s="21" t="s">
+      <c r="AZ9" s="22"/>
+      <c r="BA9" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="BB9" s="27" t="s">
+      <c r="BB9" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="BC9" s="27" t="s">
+      <c r="BC9" s="21" t="s">
         <v>89</v>
       </c>
       <c r="BJ9" s="13" t="s">
@@ -1221,8 +1303,8 @@
       <c r="BQ9" s="13"/>
       <c r="BR9" s="13"/>
     </row>
-    <row r="10" spans="2:70" ht="35.25" customHeight="1">
-      <c r="B10" s="23"/>
+    <row r="10" spans="2:70" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="35"/>
       <c r="C10" s="8" t="s">
         <v>1</v>
       </c>
@@ -1253,7 +1335,7 @@
       <c r="L10" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="M10" s="23"/>
+      <c r="M10" s="35"/>
       <c r="N10" s="8" t="s">
         <v>36</v>
       </c>
@@ -1299,7 +1381,7 @@
       <c r="AB10" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="AC10" s="31"/>
+      <c r="AC10" s="26"/>
       <c r="AD10" s="8" t="s">
         <v>67</v>
       </c>
@@ -1367,9 +1449,9 @@
       <c r="AZ10" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="BA10" s="21"/>
-      <c r="BB10" s="27"/>
-      <c r="BC10" s="27"/>
+      <c r="BA10" s="33"/>
+      <c r="BB10" s="21"/>
+      <c r="BC10" s="21"/>
       <c r="BJ10" s="8" t="s">
         <v>51</v>
       </c>
@@ -1398,7 +1480,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="2:70">
+    <row r="11" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -1433,7 +1515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:70">
+    <row r="12" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>66</v>
       </c>
@@ -1453,7 +1535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:70">
+    <row r="13" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>66</v>
       </c>
@@ -1474,7 +1556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:70">
+    <row r="14" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>94</v>
       </c>
@@ -1495,7 +1577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:70" ht="169.5" customHeight="1">
+    <row r="15" spans="2:70" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L15" s="19" t="s">
         <v>98</v>
       </c>
@@ -1532,17 +1614,20 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="14:45">
+    <row r="18" spans="14:45" x14ac:dyDescent="0.25">
       <c r="AJ18" s="10"/>
     </row>
-    <row r="20" spans="14:45">
+    <row r="20" spans="14:45" x14ac:dyDescent="0.25">
       <c r="AS20" s="15"/>
     </row>
-    <row r="26" spans="14:45">
+    <row r="26" spans="14:45" x14ac:dyDescent="0.25">
       <c r="N26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="S9:W9"/>
+    <mergeCell ref="M9:M10"/>
     <mergeCell ref="BB9:BB10"/>
     <mergeCell ref="BC9:BC10"/>
     <mergeCell ref="X9:AB9"/>
@@ -1558,9 +1643,6 @@
     <mergeCell ref="AT9:AX9"/>
     <mergeCell ref="AY9:AZ9"/>
     <mergeCell ref="BA9:BA10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="S9:W9"/>
-    <mergeCell ref="M9:M10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1568,24 +1650,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>